<commit_message>
Added arguments to NPP function: JulianDay, ProdStartDay, ProdEndDay. These arguments are used to conditionally constrain production to a specific period of the year.
Required arguments have been added to CentralFunction, CentralFunction_optim4, and modelDOC_4.

ProdStarDay and ProdEndDay must now be added to parameter files for all sites. This has been done for Vanern for testing purposes.
</commit_message>
<xml_diff>
--- a/VanernLake/ConfigurationInputsVanern.xlsx
+++ b/VanernLake/ConfigurationInputsVanern.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>g/m2/yr</t>
+  </si>
+  <si>
+    <t>#ProductionPeriod</t>
+  </si>
+  <si>
+    <t>ProdStartDay</t>
+  </si>
+  <si>
+    <t>ProdEndDay</t>
+  </si>
+  <si>
+    <t>JulianDay</t>
   </si>
 </sst>
 </file>
@@ -440,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,6 +717,33 @@
         <v>36</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <v>300</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>